<commit_message>
Adding edits to the code book.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA9F3514-7496-4A4A-8856-2B2C3854D01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55446653-49FD-6649-A87D-B88DABEA5EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Height</t>
   </si>
@@ -88,10 +88,19 @@
     <t>identified gender (male/female/other)</t>
   </si>
   <si>
-    <t>Weekly Cardio in Minutes</t>
-  </si>
-  <si>
-    <t>Daily Caffienated Beverages</t>
+    <t>Cardio</t>
+  </si>
+  <si>
+    <t>minutes of cardio in one week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whole integers </t>
+  </si>
+  <si>
+    <t>caff</t>
+  </si>
+  <si>
+    <t>number of cafienated beverages daily</t>
   </si>
 </sst>
 </file>
@@ -422,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -447,7 +456,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -692,10 +701,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -749,6 +758,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fork and pull with classmate repository
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55446653-49FD-6649-A87D-B88DABEA5EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{55446653-49FD-6649-A87D-B88DABEA5EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AA29CAF-81C9-4475-A450-0D04CA80473F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -435,14 +435,14 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="3" customWidth="1"/>
+    <col min="1" max="3" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>180</v>
       </c>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>192</v>
       </c>
@@ -493,7 +493,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>166</v>
       </c>
@@ -527,7 +527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>178</v>
       </c>
@@ -544,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>133</v>
       </c>
@@ -561,7 +561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>175</v>
       </c>
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>156</v>
       </c>
@@ -612,7 +612,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>145</v>
       </c>
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>155</v>
       </c>
@@ -646,7 +646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>165</v>
       </c>
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>154</v>
       </c>
@@ -677,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>166</v>
       </c>
@@ -707,14 +707,14 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -725,7 +725,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -736,7 +736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -747,7 +747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -758,7 +758,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -769,7 +769,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>

</xml_diff>